<commit_message>
Corrected the files, to updated ones
</commit_message>
<xml_diff>
--- a/docs/Excel_Comparing_Files/Algo1_BM3_Compare.xlsx
+++ b/docs/Excel_Comparing_Files/Algo1_BM3_Compare.xlsx
@@ -759,7 +759,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -818,6 +818,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -860,13 +869,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1172,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q146"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="F144" sqref="A1:XFD1048576"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G3" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1199,22 +1202,22 @@
     <row r="1" spans="2:16" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:16" ht="23.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
-      <c r="D2" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="24"/>
+      <c r="D2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="23"/>
-      <c r="J2" s="24"/>
-      <c r="L2" s="25" t="s">
+      <c r="I2" s="26"/>
+      <c r="J2" s="27"/>
+      <c r="L2" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="26"/>
-      <c r="N2" s="27"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="30"/>
     </row>
     <row r="3" spans="2:16" ht="18.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
@@ -1251,7 +1254,7 @@
       <c r="N3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="31" t="s">
+      <c r="P3" s="34" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1262,22 +1265,22 @@
       <c r="C4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="21">
         <v>32.104193610000003</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="14">
         <v>35.209175330000001</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="22">
         <v>685</v>
       </c>
-      <c r="H4" s="35">
+      <c r="H4" s="21">
         <v>32.104193610000003</v>
       </c>
       <c r="I4" s="14">
         <v>35.209175330000001</v>
       </c>
-      <c r="J4" s="36">
+      <c r="J4" s="22">
         <v>685</v>
       </c>
       <c r="L4" s="13">
@@ -1292,7 +1295,7 @@
         <f>ABS(J4-F4)</f>
         <v>0</v>
       </c>
-      <c r="P4" s="32"/>
+      <c r="P4" s="35"/>
     </row>
     <row r="5" spans="2:16" ht="15" x14ac:dyDescent="0.3">
       <c r="B5" s="9">
@@ -1301,13 +1304,13 @@
       <c r="C5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="13">
         <v>32.101997220000001</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="16">
         <v>35.209838099999999</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="15">
         <v>693</v>
       </c>
       <c r="H5" s="13">
@@ -1331,7 +1334,7 @@
         <f t="shared" ref="N5:N68" si="2">ABS(J5-F5)</f>
         <v>0</v>
       </c>
-      <c r="P5" s="32"/>
+      <c r="P5" s="35"/>
     </row>
     <row r="6" spans="2:16" ht="15" x14ac:dyDescent="0.3">
       <c r="B6" s="9">
@@ -1340,13 +1343,13 @@
       <c r="C6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="13">
         <v>32.104653167283601</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="16">
         <v>35.210920243042899</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="15">
         <v>691.39140401146096</v>
       </c>
       <c r="H6" s="13">
@@ -1370,7 +1373,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P6" s="32"/>
+      <c r="P6" s="35"/>
     </row>
     <row r="7" spans="2:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="9">
@@ -1379,13 +1382,13 @@
       <c r="C7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="13">
         <v>32.102838751582802</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="16">
         <v>35.209782211668802</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="15">
         <v>708.273839019913</v>
       </c>
       <c r="H7" s="13">
@@ -1409,7 +1412,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P7" s="32"/>
+      <c r="P7" s="35"/>
     </row>
     <row r="8" spans="2:16" ht="15.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="9">
@@ -1418,13 +1421,13 @@
       <c r="C8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="13">
         <v>32.104753430000002</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="16">
         <v>35.210074740000003</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="15">
         <v>689</v>
       </c>
       <c r="H8" s="13">
@@ -1448,7 +1451,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P8" s="33"/>
+      <c r="P8" s="36"/>
     </row>
     <row r="9" spans="2:16" ht="15.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B9" s="9">
@@ -1457,13 +1460,13 @@
       <c r="C9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="13">
         <v>32.102916879351497</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="16">
         <v>35.209939749115101</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="15">
         <v>698.92506640843897</v>
       </c>
       <c r="H9" s="13">
@@ -1495,13 +1498,13 @@
       <c r="C10" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="13">
         <v>32.103653587234099</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="16">
         <v>35.210101386364499</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="15">
         <v>710.67107941880602</v>
       </c>
       <c r="H10" s="13">
@@ -1533,13 +1536,13 @@
       <c r="C11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="13">
         <v>32.102624499337601</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="16">
         <v>35.209874406505499</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="15">
         <v>707.91417060501601</v>
       </c>
       <c r="H11" s="13">
@@ -1571,13 +1574,13 @@
       <c r="C12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="13">
         <v>32.102954570000001</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="16">
         <v>35.208804299999997</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="15">
         <v>686</v>
       </c>
       <c r="H12" s="13">
@@ -1609,13 +1612,13 @@
       <c r="C13" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="13">
         <v>32.103156517673902</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="16">
         <v>35.2095290500204</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F13" s="15">
         <v>690.80821434733502</v>
       </c>
       <c r="H13" s="13">
@@ -1647,13 +1650,13 @@
       <c r="C14" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="13">
         <v>32.103195765488202</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="16">
         <v>35.209881768789003</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="15">
         <v>701.71077604122502</v>
       </c>
       <c r="H14" s="13">
@@ -1685,13 +1688,13 @@
       <c r="C15" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="13">
         <v>32.102984973516897</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="16">
         <v>35.209664769476603</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="15">
         <v>704.82769153732204</v>
       </c>
       <c r="H15" s="13">
@@ -1723,13 +1726,13 @@
       <c r="C16" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="13">
         <v>32.103376616352399</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="16">
         <v>35.209958682147402</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="15">
         <v>698.31960846040795</v>
       </c>
       <c r="H16" s="13">
@@ -1761,13 +1764,13 @@
       <c r="C17" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="13">
         <v>32.103327865979097</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="16">
         <v>35.209655511021197</v>
       </c>
-      <c r="F17" s="16">
+      <c r="F17" s="15">
         <v>704.83978952370501</v>
       </c>
       <c r="H17" s="13">
@@ -1799,13 +1802,13 @@
       <c r="C18" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="13">
         <v>32.104849817715397</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="16">
         <v>35.211049231927298</v>
       </c>
-      <c r="F18" s="16">
+      <c r="F18" s="15">
         <v>693.987986415931</v>
       </c>
       <c r="H18" s="13">
@@ -1837,13 +1840,13 @@
       <c r="C19" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="13">
         <v>32.1022050142574</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="16">
         <v>35.209365924973298</v>
       </c>
-      <c r="F19" s="16">
+      <c r="F19" s="15">
         <v>689.61157654226895</v>
       </c>
       <c r="H19" s="13">
@@ -1875,13 +1878,13 @@
       <c r="C20" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="13">
         <v>32.102192340000002</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="16">
         <v>35.209466280000001</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F20" s="15">
         <v>690</v>
       </c>
       <c r="H20" s="13">
@@ -1913,13 +1916,13 @@
       <c r="C21" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="13">
         <v>32.102748690917103</v>
       </c>
-      <c r="E21" s="11">
+      <c r="E21" s="16">
         <v>35.2098294611611</v>
       </c>
-      <c r="F21" s="16">
+      <c r="F21" s="15">
         <v>708.11433820273601</v>
       </c>
       <c r="H21" s="13">
@@ -1951,13 +1954,13 @@
       <c r="C22" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D22" s="13">
         <v>32.102702185088297</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E22" s="16">
         <v>35.209827552141299</v>
       </c>
-      <c r="F22" s="16">
+      <c r="F22" s="15">
         <v>710.11101864433601</v>
       </c>
       <c r="H22" s="13">
@@ -1989,14 +1992,14 @@
       <c r="C23" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="16">
-        <v>32.102632083867199</v>
-      </c>
-      <c r="E23" s="11">
-        <v>35.2089916185733</v>
-      </c>
-      <c r="F23" s="16">
-        <v>687.55122368918398</v>
+      <c r="D23" s="13">
+        <v>32.102787023903097</v>
+      </c>
+      <c r="E23" s="16">
+        <v>35.209009024146297</v>
+      </c>
+      <c r="F23" s="15">
+        <v>687.36554568333895</v>
       </c>
       <c r="H23" s="13">
         <v>32.102538763935897</v>
@@ -2009,15 +2012,15 @@
       </c>
       <c r="L23" s="13">
         <f t="shared" si="0"/>
-        <v>9.3319931302460191E-5</v>
+        <v>2.4825996720068133E-4</v>
       </c>
       <c r="M23" s="16">
         <f t="shared" si="1"/>
-        <v>4.3557958299800248E-5</v>
+        <v>2.6152385302680159E-5</v>
       </c>
       <c r="N23" s="15">
         <f t="shared" si="2"/>
-        <v>0.59450748036306322</v>
+        <v>0.78018548620809725</v>
       </c>
     </row>
     <row r="24" spans="2:14" ht="15" x14ac:dyDescent="0.3">
@@ -2027,13 +2030,13 @@
       <c r="C24" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="16">
+      <c r="D24" s="13">
         <v>32.103109806320099</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="16">
         <v>35.209879561491803</v>
       </c>
-      <c r="F24" s="16">
+      <c r="F24" s="15">
         <v>701.81798145203197</v>
       </c>
       <c r="H24" s="13">
@@ -2065,13 +2068,13 @@
       <c r="C25" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="16">
+      <c r="D25" s="13">
         <v>32.1029604932571</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="16">
         <v>35.209699133932197</v>
       </c>
-      <c r="F25" s="16">
+      <c r="F25" s="15">
         <v>702.14287995796701</v>
       </c>
       <c r="H25" s="13">
@@ -2103,13 +2106,13 @@
       <c r="C26" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="16">
+      <c r="D26" s="13">
         <v>32.102599911192797</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26" s="16">
         <v>35.2090994031796</v>
       </c>
-      <c r="F26" s="16">
+      <c r="F26" s="15">
         <v>688.81976645841405</v>
       </c>
       <c r="H26" s="13">
@@ -2141,13 +2144,13 @@
       <c r="C27" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="16">
+      <c r="D27" s="13">
         <v>32.10244119</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E27" s="16">
         <v>35.208849139999998</v>
       </c>
-      <c r="F27" s="16">
+      <c r="F27" s="15">
         <v>686</v>
       </c>
       <c r="H27" s="13">
@@ -2179,13 +2182,13 @@
       <c r="C28" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="16">
+      <c r="D28" s="13">
         <v>32.103851797833997</v>
       </c>
-      <c r="E28" s="11">
+      <c r="E28" s="16">
         <v>35.210022168124198</v>
       </c>
-      <c r="F28" s="16">
+      <c r="F28" s="15">
         <v>696.25303092692604</v>
       </c>
       <c r="H28" s="13">
@@ -2217,13 +2220,13 @@
       <c r="C29" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="16">
+      <c r="D29" s="13">
         <v>32.1037119778373</v>
       </c>
-      <c r="E29" s="11">
+      <c r="E29" s="16">
         <v>35.210039357346098</v>
       </c>
-      <c r="F29" s="16">
+      <c r="F29" s="15">
         <v>711.07537640210603</v>
       </c>
       <c r="H29" s="13">
@@ -2255,13 +2258,13 @@
       <c r="C30" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="16">
+      <c r="D30" s="13">
         <v>32.102505779588199</v>
       </c>
-      <c r="E30" s="11">
+      <c r="E30" s="16">
         <v>35.209555310518901</v>
       </c>
-      <c r="F30" s="16">
+      <c r="F30" s="15">
         <v>690.85561032183205</v>
       </c>
       <c r="H30" s="13">
@@ -2293,13 +2296,13 @@
       <c r="C31" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="16">
+      <c r="D31" s="13">
         <v>32.102380846733197</v>
       </c>
-      <c r="E31" s="11">
+      <c r="E31" s="16">
         <v>35.210006539970799</v>
       </c>
-      <c r="F31" s="16">
+      <c r="F31" s="15">
         <v>712.19374266854902</v>
       </c>
       <c r="H31" s="13">
@@ -2331,13 +2334,13 @@
       <c r="C32" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="16">
+      <c r="D32" s="13">
         <v>32.104222915734397</v>
       </c>
-      <c r="E32" s="11">
+      <c r="E32" s="16">
         <v>35.209310300322201</v>
       </c>
-      <c r="F32" s="16">
+      <c r="F32" s="15">
         <v>686.46346353779802</v>
       </c>
       <c r="H32" s="13">
@@ -2369,13 +2372,13 @@
       <c r="C33" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="16">
+      <c r="D33" s="13">
         <v>32.104831794886799</v>
       </c>
-      <c r="E33" s="11">
+      <c r="E33" s="16">
         <v>35.210369626968301</v>
       </c>
-      <c r="F33" s="16">
+      <c r="F33" s="15">
         <v>686.99999999999898</v>
       </c>
       <c r="H33" s="13">
@@ -2407,13 +2410,13 @@
       <c r="C34" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="16">
+      <c r="D34" s="13">
         <v>32.102423595820198</v>
       </c>
-      <c r="E34" s="11">
+      <c r="E34" s="16">
         <v>35.209678671248398</v>
       </c>
-      <c r="F34" s="16">
+      <c r="F34" s="15">
         <v>691.26509454625102</v>
       </c>
       <c r="H34" s="13">
@@ -2445,13 +2448,13 @@
       <c r="C35" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="16">
+      <c r="D35" s="13">
         <v>32.102461204005103</v>
       </c>
-      <c r="E35" s="11">
+      <c r="E35" s="16">
         <v>35.209976991172901</v>
       </c>
-      <c r="F35" s="16">
+      <c r="F35" s="15">
         <v>711.92892574918699</v>
       </c>
       <c r="H35" s="13">
@@ -2483,13 +2486,13 @@
       <c r="C36" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="16">
+      <c r="D36" s="13">
         <v>32.104433960398701</v>
       </c>
-      <c r="E36" s="11">
+      <c r="E36" s="16">
         <v>35.210832068376803</v>
       </c>
-      <c r="F36" s="16">
+      <c r="F36" s="15">
         <v>694.78030591279196</v>
       </c>
       <c r="H36" s="13">
@@ -2521,13 +2524,13 @@
       <c r="C37" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D37" s="16">
+      <c r="D37" s="13">
         <v>32.104857024876502</v>
       </c>
-      <c r="E37" s="11">
+      <c r="E37" s="16">
         <v>35.210807843935399</v>
       </c>
-      <c r="F37" s="16">
+      <c r="F37" s="15">
         <v>690.02339101292603</v>
       </c>
       <c r="H37" s="13">
@@ -2559,13 +2562,13 @@
       <c r="C38" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="16">
+      <c r="D38" s="13">
         <v>32.104883685804303</v>
       </c>
-      <c r="E38" s="11">
+      <c r="E38" s="16">
         <v>35.210927889966598</v>
       </c>
-      <c r="F38" s="16">
+      <c r="F38" s="15">
         <v>691.41920448644998</v>
       </c>
       <c r="H38" s="13">
@@ -2597,13 +2600,13 @@
       <c r="C39" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="16">
+      <c r="D39" s="13">
         <v>32.104588311061903</v>
       </c>
-      <c r="E39" s="11">
+      <c r="E39" s="16">
         <v>35.211044870353902</v>
       </c>
-      <c r="F39" s="16">
+      <c r="F39" s="15">
         <v>692.79646017699099</v>
       </c>
       <c r="H39" s="13">
@@ -2635,13 +2638,13 @@
       <c r="C40" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D40" s="16">
+      <c r="D40" s="13">
         <v>32.103053060000001</v>
       </c>
-      <c r="E40" s="11">
+      <c r="E40" s="16">
         <v>35.209784460000002</v>
       </c>
-      <c r="F40" s="16">
+      <c r="F40" s="15">
         <v>693</v>
       </c>
       <c r="H40" s="13">
@@ -2673,13 +2676,13 @@
       <c r="C41" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D41" s="16">
+      <c r="D41" s="13">
         <v>32.102991836947702</v>
       </c>
-      <c r="E41" s="11">
+      <c r="E41" s="16">
         <v>35.2096724012114</v>
       </c>
-      <c r="F41" s="16">
+      <c r="F41" s="15">
         <v>704.95677573850503</v>
       </c>
       <c r="H41" s="13">
@@ -2711,13 +2714,13 @@
       <c r="C42" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D42" s="16">
+      <c r="D42" s="13">
         <v>32.103603158327402</v>
       </c>
-      <c r="E42" s="11">
+      <c r="E42" s="16">
         <v>35.210005054877499</v>
       </c>
-      <c r="F42" s="16">
+      <c r="F42" s="15">
         <v>710.581462210155</v>
       </c>
       <c r="H42" s="13">
@@ -2749,13 +2752,13 @@
       <c r="C43" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D43" s="16">
+      <c r="D43" s="13">
         <v>32.103510723274503</v>
       </c>
-      <c r="E43" s="11">
+      <c r="E43" s="16">
         <v>35.209905544936397</v>
       </c>
-      <c r="F43" s="16">
+      <c r="F43" s="15">
         <v>710.41941074451802</v>
       </c>
       <c r="H43" s="13">
@@ -2787,13 +2790,13 @@
       <c r="C44" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D44" s="16">
+      <c r="D44" s="13">
         <v>32.104573925168502</v>
       </c>
-      <c r="E44" s="11">
+      <c r="E44" s="16">
         <v>35.211212793696603</v>
       </c>
-      <c r="F44" s="16">
+      <c r="F44" s="15">
         <v>694.37313278333295</v>
       </c>
       <c r="H44" s="13">
@@ -2825,13 +2828,13 @@
       <c r="C45" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D45" s="16">
+      <c r="D45" s="13">
         <v>32.103838000233402</v>
       </c>
-      <c r="E45" s="11">
+      <c r="E45" s="16">
         <v>35.210004707997903</v>
       </c>
-      <c r="F45" s="16">
+      <c r="F45" s="15">
         <v>698.69085575894701</v>
       </c>
       <c r="H45" s="13">
@@ -2863,13 +2866,13 @@
       <c r="C46" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D46" s="16">
+      <c r="D46" s="13">
         <v>32.103510723274503</v>
       </c>
-      <c r="E46" s="11">
+      <c r="E46" s="16">
         <v>35.209905544936397</v>
       </c>
-      <c r="F46" s="16">
+      <c r="F46" s="15">
         <v>710.41941074451802</v>
       </c>
       <c r="H46" s="13">
@@ -2901,13 +2904,13 @@
       <c r="C47" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="D47" s="16">
+      <c r="D47" s="13">
         <v>32.104814920000003</v>
       </c>
-      <c r="E47" s="11">
+      <c r="E47" s="16">
         <v>35.211453900000002</v>
       </c>
-      <c r="F47" s="16">
+      <c r="F47" s="15">
         <v>695</v>
       </c>
       <c r="H47" s="13">
@@ -2939,14 +2942,14 @@
       <c r="C48" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D48" s="16">
-        <v>32.104358953660302</v>
-      </c>
-      <c r="E48" s="11">
-        <v>35.209761250813102</v>
-      </c>
-      <c r="F48" s="16">
-        <v>686.30718609537405</v>
+      <c r="D48" s="13">
+        <v>32.104236871108903</v>
+      </c>
+      <c r="E48" s="16">
+        <v>35.209664232168599</v>
+      </c>
+      <c r="F48" s="15">
+        <v>685.47381395399805</v>
       </c>
       <c r="H48" s="13">
         <v>32.104242165845498</v>
@@ -2959,15 +2962,15 @@
       </c>
       <c r="L48" s="13">
         <f t="shared" si="0"/>
-        <v>1.1678781480384259E-4</v>
+        <v>5.2947365958289083E-6</v>
       </c>
       <c r="M48" s="16">
         <f t="shared" si="1"/>
-        <v>1.6636263229941051E-4</v>
+        <v>6.9343987796344209E-5</v>
       </c>
       <c r="N48" s="15">
         <f t="shared" si="2"/>
-        <v>6.0315759233958488E-2</v>
+        <v>0.89368790060996162</v>
       </c>
     </row>
     <row r="49" spans="2:14" ht="15" x14ac:dyDescent="0.3">
@@ -2977,13 +2980,13 @@
       <c r="C49" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D49" s="16">
+      <c r="D49" s="13">
         <v>32.104759284034699</v>
       </c>
-      <c r="E49" s="11">
+      <c r="E49" s="16">
         <v>35.210386626142601</v>
       </c>
-      <c r="F49" s="16">
+      <c r="F49" s="15">
         <v>690.87844277559702</v>
       </c>
       <c r="H49" s="13">
@@ -3015,14 +3018,14 @@
       <c r="C50" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D50" s="16">
-        <v>32.103475105323199</v>
-      </c>
-      <c r="E50" s="11">
-        <v>35.210029559728703</v>
-      </c>
-      <c r="F50" s="16">
-        <v>704.28352912806997</v>
+      <c r="D50" s="13">
+        <v>32.103547178621596</v>
+      </c>
+      <c r="E50" s="16">
+        <v>35.210137634907497</v>
+      </c>
+      <c r="F50" s="15">
+        <v>698.51832519100196</v>
       </c>
       <c r="H50" s="13">
         <v>32.103533681273099</v>
@@ -3035,15 +3038,15 @@
       </c>
       <c r="L50" s="13">
         <f t="shared" si="0"/>
-        <v>5.8575949900330215E-5</v>
+        <v>1.3497348497537587E-5</v>
       </c>
       <c r="M50" s="16">
         <f t="shared" si="1"/>
-        <v>7.1108786599438645E-5</v>
+        <v>1.7918396539329251E-4</v>
       </c>
       <c r="N50" s="15">
         <f t="shared" si="2"/>
-        <v>1.652571260406944</v>
+        <v>4.1126326766610646</v>
       </c>
     </row>
     <row r="51" spans="2:14" ht="15" x14ac:dyDescent="0.3">
@@ -3053,13 +3056,13 @@
       <c r="C51" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D51" s="16">
+      <c r="D51" s="13">
         <v>32.103585082541898</v>
       </c>
-      <c r="E51" s="11">
+      <c r="E51" s="16">
         <v>35.210396203216398</v>
       </c>
-      <c r="F51" s="16">
+      <c r="F51" s="15">
         <v>699.193327757254</v>
       </c>
       <c r="H51" s="13">
@@ -3091,13 +3094,13 @@
       <c r="C52" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="D52" s="16">
+      <c r="D52" s="13">
         <v>32.102545849511799</v>
       </c>
-      <c r="E52" s="11">
+      <c r="E52" s="16">
         <v>35.209411778437001</v>
       </c>
-      <c r="F52" s="16">
+      <c r="F52" s="15">
         <v>690.70036819926702</v>
       </c>
       <c r="H52" s="13">
@@ -3129,13 +3132,13 @@
       <c r="C53" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D53" s="16">
+      <c r="D53" s="13">
         <v>32.102823620000002</v>
       </c>
-      <c r="E53" s="11">
+      <c r="E53" s="16">
         <v>35.208718990000001</v>
       </c>
-      <c r="F53" s="16">
+      <c r="F53" s="15">
         <v>688</v>
       </c>
       <c r="H53" s="13">
@@ -3167,13 +3170,13 @@
       <c r="C54" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D54" s="16">
+      <c r="D54" s="13">
         <v>32.103856012910001</v>
       </c>
-      <c r="E54" s="11">
+      <c r="E54" s="16">
         <v>35.209093699346397</v>
       </c>
-      <c r="F54" s="16">
+      <c r="F54" s="15">
         <v>687</v>
       </c>
       <c r="H54" s="13">
@@ -3205,13 +3208,13 @@
       <c r="C55" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D55" s="16">
+      <c r="D55" s="13">
         <v>32.103709233473602</v>
       </c>
-      <c r="E55" s="11">
+      <c r="E55" s="16">
         <v>35.209461735434303</v>
       </c>
-      <c r="F55" s="16">
+      <c r="F55" s="15">
         <v>698.19771675153595</v>
       </c>
       <c r="H55" s="13">
@@ -3243,13 +3246,13 @@
       <c r="C56" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D56" s="16">
+      <c r="D56" s="13">
         <v>32.103399625399199</v>
       </c>
-      <c r="E56" s="11">
+      <c r="E56" s="16">
         <v>35.208874501746202</v>
       </c>
-      <c r="F56" s="16">
+      <c r="F56" s="15">
         <v>685.700714863043</v>
       </c>
       <c r="H56" s="13">
@@ -3281,13 +3284,13 @@
       <c r="C57" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D57" s="16">
+      <c r="D57" s="13">
         <v>32.103749324615301</v>
       </c>
-      <c r="E57" s="11">
+      <c r="E57" s="16">
         <v>35.210097366410899</v>
       </c>
-      <c r="F57" s="16">
+      <c r="F57" s="15">
         <v>711.04240246276004</v>
       </c>
       <c r="H57" s="13">
@@ -3319,13 +3322,13 @@
       <c r="C58" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D58" s="16">
+      <c r="D58" s="13">
         <v>32.102587651350298</v>
       </c>
-      <c r="E58" s="11">
+      <c r="E58" s="16">
         <v>35.209114654448697</v>
       </c>
-      <c r="F58" s="16">
+      <c r="F58" s="15">
         <v>688.10250513331505</v>
       </c>
       <c r="H58" s="13">
@@ -3357,13 +3360,13 @@
       <c r="C59" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D59" s="16">
+      <c r="D59" s="13">
         <v>32.104862322887598</v>
       </c>
-      <c r="E59" s="11">
+      <c r="E59" s="16">
         <v>35.2107809414711</v>
       </c>
-      <c r="F59" s="16">
+      <c r="F59" s="15">
         <v>692.76483607691205</v>
       </c>
       <c r="H59" s="13">
@@ -3395,13 +3398,13 @@
       <c r="C60" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="D60" s="16">
+      <c r="D60" s="13">
         <v>32.104759929925898</v>
       </c>
-      <c r="E60" s="11">
+      <c r="E60" s="16">
         <v>35.210309410163198</v>
       </c>
-      <c r="F60" s="16">
+      <c r="F60" s="15">
         <v>687.28630716266605</v>
       </c>
       <c r="H60" s="13">
@@ -3433,13 +3436,13 @@
       <c r="C61" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D61" s="16">
+      <c r="D61" s="13">
         <v>32.104198361484897</v>
       </c>
-      <c r="E61" s="11">
+      <c r="E61" s="16">
         <v>35.209193501392399</v>
       </c>
-      <c r="F61" s="16">
+      <c r="F61" s="15">
         <v>685.53703551292301</v>
       </c>
       <c r="H61" s="13">
@@ -3471,13 +3474,13 @@
       <c r="C62" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D62" s="16">
+      <c r="D62" s="13">
         <v>32.10476714</v>
       </c>
-      <c r="E62" s="11">
+      <c r="E62" s="16">
         <v>35.211515599999998</v>
       </c>
-      <c r="F62" s="16">
+      <c r="F62" s="15">
         <v>696</v>
       </c>
       <c r="H62" s="13">
@@ -3509,13 +3512,13 @@
       <c r="C63" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D63" s="16">
+      <c r="D63" s="13">
         <v>32.103231978973199</v>
       </c>
-      <c r="E63" s="11">
+      <c r="E63" s="16">
         <v>35.208810181426699</v>
       </c>
-      <c r="F63" s="16">
+      <c r="F63" s="15">
         <v>686</v>
       </c>
       <c r="H63" s="13">
@@ -3547,13 +3550,13 @@
       <c r="C64" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D64" s="16">
+      <c r="D64" s="13">
         <v>32.103409981137098</v>
       </c>
-      <c r="E64" s="11">
+      <c r="E64" s="16">
         <v>35.209694768890699</v>
       </c>
-      <c r="F64" s="16">
+      <c r="F64" s="15">
         <v>704.41032680407295</v>
       </c>
       <c r="H64" s="13">
@@ -3585,13 +3588,13 @@
       <c r="C65" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="D65" s="16">
+      <c r="D65" s="13">
         <v>32.103401442087602</v>
       </c>
-      <c r="E65" s="11">
+      <c r="E65" s="16">
         <v>35.210113015183197</v>
       </c>
-      <c r="F65" s="16">
+      <c r="F65" s="15">
         <v>700.94453604110402</v>
       </c>
       <c r="H65" s="13">
@@ -3623,13 +3626,13 @@
       <c r="C66" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D66" s="16">
+      <c r="D66" s="13">
         <v>32.1029604932571</v>
       </c>
-      <c r="E66" s="11">
+      <c r="E66" s="16">
         <v>35.209699133932197</v>
       </c>
-      <c r="F66" s="16">
+      <c r="F66" s="15">
         <v>702.14287995796701</v>
       </c>
       <c r="H66" s="13">
@@ -3661,13 +3664,13 @@
       <c r="C67" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="D67" s="16">
+      <c r="D67" s="13">
         <v>32.103718923267103</v>
       </c>
-      <c r="E67" s="11">
+      <c r="E67" s="16">
         <v>35.2103601271846</v>
       </c>
-      <c r="F67" s="16">
+      <c r="F67" s="15">
         <v>697.52993904625305</v>
       </c>
       <c r="H67" s="13">
@@ -3699,13 +3702,13 @@
       <c r="C68" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="D68" s="16">
+      <c r="D68" s="13">
         <v>32.102751834050999</v>
       </c>
-      <c r="E68" s="11">
+      <c r="E68" s="16">
         <v>35.209488976149103</v>
       </c>
-      <c r="F68" s="16">
+      <c r="F68" s="15">
         <v>696.46163260095796</v>
       </c>
       <c r="H68" s="13">
@@ -3737,13 +3740,13 @@
       <c r="C69" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D69" s="16">
+      <c r="D69" s="13">
         <v>32.103245195129901</v>
       </c>
-      <c r="E69" s="11">
+      <c r="E69" s="16">
         <v>35.2097792384168</v>
       </c>
-      <c r="F69" s="16">
+      <c r="F69" s="15">
         <v>707.25042391811201</v>
       </c>
       <c r="H69" s="13">
@@ -3775,13 +3778,13 @@
       <c r="C70" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D70" s="16">
+      <c r="D70" s="13">
         <v>32.102475235809301</v>
       </c>
-      <c r="E70" s="11">
+      <c r="E70" s="16">
         <v>35.208922693241597</v>
       </c>
-      <c r="F70" s="16">
+      <c r="F70" s="15">
         <v>686.50663865556498</v>
       </c>
       <c r="H70" s="13">
@@ -3813,13 +3816,13 @@
       <c r="C71" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D71" s="16">
+      <c r="D71" s="13">
         <v>32.102850495732604</v>
       </c>
-      <c r="E71" s="11">
+      <c r="E71" s="16">
         <v>35.208877284273498</v>
       </c>
-      <c r="F71" s="16">
+      <c r="F71" s="15">
         <v>686.31181773770504</v>
       </c>
       <c r="H71" s="13">
@@ -3851,13 +3854,13 @@
       <c r="C72" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D72" s="16">
+      <c r="D72" s="13">
         <v>32.102823620000002</v>
       </c>
-      <c r="E72" s="11">
+      <c r="E72" s="16">
         <v>35.208718990000001</v>
       </c>
-      <c r="F72" s="16">
+      <c r="F72" s="15">
         <v>688</v>
       </c>
       <c r="H72" s="13">
@@ -3889,13 +3892,13 @@
       <c r="C73" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D73" s="16">
+      <c r="D73" s="13">
         <v>32.10476714</v>
       </c>
-      <c r="E73" s="11">
+      <c r="E73" s="16">
         <v>35.211515599999998</v>
       </c>
-      <c r="F73" s="16">
+      <c r="F73" s="15">
         <v>696</v>
       </c>
       <c r="H73" s="13">
@@ -3927,13 +3930,13 @@
       <c r="C74" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="D74" s="16">
+      <c r="D74" s="13">
         <v>32.102963777631302</v>
       </c>
-      <c r="E74" s="11">
+      <c r="E74" s="16">
         <v>35.209689677091099</v>
       </c>
-      <c r="F74" s="16">
+      <c r="F74" s="15">
         <v>704.74718563256795</v>
       </c>
       <c r="H74" s="13">
@@ -3965,13 +3968,13 @@
       <c r="C75" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="D75" s="16">
+      <c r="D75" s="13">
         <v>32.103371135376499</v>
       </c>
-      <c r="E75" s="11">
+      <c r="E75" s="16">
         <v>35.209710253406399</v>
       </c>
-      <c r="F75" s="16">
+      <c r="F75" s="15">
         <v>704.100695841272</v>
       </c>
       <c r="H75" s="13">
@@ -4003,13 +4006,13 @@
       <c r="C76" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="D76" s="16">
+      <c r="D76" s="13">
         <v>32.102622609262397</v>
       </c>
-      <c r="E76" s="11">
+      <c r="E76" s="16">
         <v>35.2098928453102</v>
       </c>
-      <c r="F76" s="16">
+      <c r="F76" s="15">
         <v>707.95932165568502</v>
       </c>
       <c r="H76" s="13">
@@ -4041,13 +4044,13 @@
       <c r="C77" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="D77" s="16">
+      <c r="D77" s="13">
         <v>32.1029604932571</v>
       </c>
-      <c r="E77" s="11">
+      <c r="E77" s="16">
         <v>35.209699133932197</v>
       </c>
-      <c r="F77" s="16">
+      <c r="F77" s="15">
         <v>702.14287995796701</v>
       </c>
       <c r="H77" s="13">
@@ -4079,13 +4082,13 @@
       <c r="C78" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D78" s="16">
+      <c r="D78" s="13">
         <v>32.103039854798702</v>
       </c>
-      <c r="E78" s="11">
+      <c r="E78" s="16">
         <v>35.209688265555201</v>
       </c>
-      <c r="F78" s="16">
+      <c r="F78" s="15">
         <v>703.11594160033997</v>
       </c>
       <c r="H78" s="13">
@@ -4117,13 +4120,13 @@
       <c r="C79" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D79" s="16">
+      <c r="D79" s="13">
         <v>32.102380846733197</v>
       </c>
-      <c r="E79" s="11">
+      <c r="E79" s="16">
         <v>35.210006539970799</v>
       </c>
-      <c r="F79" s="16">
+      <c r="F79" s="15">
         <v>712.19374266854902</v>
       </c>
       <c r="H79" s="13">
@@ -4155,13 +4158,13 @@
       <c r="C80" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D80" s="16">
+      <c r="D80" s="13">
         <v>32.102380846733197</v>
       </c>
-      <c r="E80" s="11">
+      <c r="E80" s="16">
         <v>35.210006539970799</v>
       </c>
-      <c r="F80" s="16">
+      <c r="F80" s="15">
         <v>712.19374266854902</v>
       </c>
       <c r="H80" s="13">
@@ -4193,13 +4196,13 @@
       <c r="C81" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D81" s="16">
+      <c r="D81" s="13">
         <v>32.104236110000002</v>
       </c>
-      <c r="E81" s="11">
+      <c r="E81" s="16">
         <v>35.211383189999999</v>
       </c>
-      <c r="F81" s="16">
+      <c r="F81" s="15">
         <v>700</v>
       </c>
       <c r="H81" s="13">
@@ -4231,13 +4234,13 @@
       <c r="C82" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="D82" s="16">
+      <c r="D82" s="13">
         <v>32.102958014085502</v>
       </c>
-      <c r="E82" s="11">
+      <c r="E82" s="16">
         <v>35.209677740279702</v>
       </c>
-      <c r="F82" s="16">
+      <c r="F82" s="15">
         <v>707.84788686281604</v>
       </c>
       <c r="H82" s="13">
@@ -4269,13 +4272,13 @@
       <c r="C83" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D83" s="16">
+      <c r="D83" s="13">
         <v>32.103422735825902</v>
       </c>
-      <c r="E83" s="11">
+      <c r="E83" s="16">
         <v>35.209711901095503</v>
       </c>
-      <c r="F83" s="16">
+      <c r="F83" s="15">
         <v>704.24502290678004</v>
       </c>
       <c r="H83" s="13">
@@ -4307,13 +4310,13 @@
       <c r="C84" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D84" s="16">
+      <c r="D84" s="13">
         <v>32.103539043883202</v>
       </c>
-      <c r="E84" s="11">
+      <c r="E84" s="16">
         <v>35.209946390164198</v>
       </c>
-      <c r="F84" s="16">
+      <c r="F84" s="15">
         <v>710.47704989135002</v>
       </c>
       <c r="H84" s="13">
@@ -4345,13 +4348,13 @@
       <c r="C85" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D85" s="16">
+      <c r="D85" s="13">
         <v>32.104666270000003</v>
       </c>
-      <c r="E85" s="11">
+      <c r="E85" s="16">
         <v>35.209909359999997</v>
       </c>
-      <c r="F85" s="16">
+      <c r="F85" s="15">
         <v>687</v>
       </c>
       <c r="H85" s="13">
@@ -4383,13 +4386,13 @@
       <c r="C86" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D86" s="16">
+      <c r="D86" s="13">
         <v>32.102684896190503</v>
       </c>
-      <c r="E86" s="11">
+      <c r="E86" s="16">
         <v>35.2097954194316</v>
       </c>
-      <c r="F86" s="16">
+      <c r="F86" s="15">
         <v>707.82804725910898</v>
       </c>
       <c r="H86" s="13">
@@ -4421,13 +4424,13 @@
       <c r="C87" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="D87" s="16">
+      <c r="D87" s="13">
         <v>32.103810095687699</v>
       </c>
-      <c r="E87" s="11">
+      <c r="E87" s="16">
         <v>35.210283621423898</v>
       </c>
-      <c r="F87" s="16">
+      <c r="F87" s="15">
         <v>710.90612609066795</v>
       </c>
       <c r="H87" s="13">
@@ -4459,13 +4462,13 @@
       <c r="C88" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D88" s="16">
+      <c r="D88" s="13">
         <v>32.103749324615301</v>
       </c>
-      <c r="E88" s="11">
+      <c r="E88" s="16">
         <v>35.210097366410899</v>
       </c>
-      <c r="F88" s="16">
+      <c r="F88" s="15">
         <v>711.04240246276004</v>
       </c>
       <c r="H88" s="13">
@@ -4497,13 +4500,13 @@
       <c r="C89" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="D89" s="16">
+      <c r="D89" s="13">
         <v>32.103126799123601</v>
       </c>
-      <c r="E89" s="11">
+      <c r="E89" s="16">
         <v>35.209182330357301</v>
       </c>
-      <c r="F89" s="16">
+      <c r="F89" s="15">
         <v>695.57060690669698</v>
       </c>
       <c r="H89" s="13">
@@ -4535,13 +4538,13 @@
       <c r="C90" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="D90" s="16">
+      <c r="D90" s="13">
         <v>32.103810095687699</v>
       </c>
-      <c r="E90" s="11">
+      <c r="E90" s="16">
         <v>35.210283621423898</v>
       </c>
-      <c r="F90" s="16">
+      <c r="F90" s="15">
         <v>710.90612609066795</v>
       </c>
       <c r="H90" s="13">
@@ -4573,13 +4576,13 @@
       <c r="C91" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="D91" s="16">
+      <c r="D91" s="13">
         <v>32.1030208456623</v>
       </c>
-      <c r="E91" s="11">
+      <c r="E91" s="16">
         <v>35.209664369663599</v>
       </c>
-      <c r="F91" s="16">
+      <c r="F91" s="15">
         <v>702.83023486280194</v>
       </c>
       <c r="H91" s="13">
@@ -4611,13 +4614,13 @@
       <c r="C92" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D92" s="16">
+      <c r="D92" s="13">
         <v>32.103422735825902</v>
       </c>
-      <c r="E92" s="11">
+      <c r="E92" s="16">
         <v>35.209711901095503</v>
       </c>
-      <c r="F92" s="16">
+      <c r="F92" s="15">
         <v>704.24502290678004</v>
       </c>
       <c r="H92" s="13">
@@ -4649,13 +4652,13 @@
       <c r="C93" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D93" s="16">
+      <c r="D93" s="13">
         <v>32.1027508529287</v>
       </c>
-      <c r="E93" s="11">
+      <c r="E93" s="16">
         <v>35.209759558946303</v>
       </c>
-      <c r="F93" s="16">
+      <c r="F93" s="15">
         <v>707.65276648020199</v>
       </c>
       <c r="H93" s="13">
@@ -4687,13 +4690,13 @@
       <c r="C94" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="D94" s="16">
+      <c r="D94" s="13">
         <v>32.103409981137098</v>
       </c>
-      <c r="E94" s="11">
+      <c r="E94" s="16">
         <v>35.209694768890699</v>
       </c>
-      <c r="F94" s="16">
+      <c r="F94" s="15">
         <v>704.41032680407295</v>
       </c>
       <c r="H94" s="13">
@@ -4725,13 +4728,13 @@
       <c r="C95" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="D95" s="16">
+      <c r="D95" s="13">
         <v>32.103269810776702</v>
       </c>
-      <c r="E95" s="11">
+      <c r="E95" s="16">
         <v>35.209780490729003</v>
       </c>
-      <c r="F95" s="16">
+      <c r="F95" s="15">
         <v>710.87795863936799</v>
       </c>
       <c r="H95" s="13">
@@ -4763,13 +4766,13 @@
       <c r="C96" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D96" s="16">
+      <c r="D96" s="13">
         <v>32.1039348867765</v>
       </c>
-      <c r="E96" s="11">
+      <c r="E96" s="16">
         <v>35.210588343327899</v>
       </c>
-      <c r="F96" s="16">
+      <c r="F96" s="15">
         <v>702.27584352025406</v>
       </c>
       <c r="H96" s="13">
@@ -4801,13 +4804,13 @@
       <c r="C97" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D97" s="16">
+      <c r="D97" s="13">
         <v>32.103698614805801</v>
       </c>
-      <c r="E97" s="11">
+      <c r="E97" s="16">
         <v>35.210175411817801</v>
       </c>
-      <c r="F97" s="16">
+      <c r="F97" s="15">
         <v>710.74852344698797</v>
       </c>
       <c r="H97" s="13">
@@ -4839,13 +4842,13 @@
       <c r="C98" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D98" s="16">
+      <c r="D98" s="13">
         <v>32.103927385567097</v>
       </c>
-      <c r="E98" s="11">
+      <c r="E98" s="16">
         <v>35.2105669454889</v>
       </c>
-      <c r="F98" s="16">
+      <c r="F98" s="15">
         <v>702.57386385530594</v>
       </c>
       <c r="H98" s="13">
@@ -4877,13 +4880,13 @@
       <c r="C99" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="D99" s="16">
+      <c r="D99" s="13">
         <v>32.103754328139701</v>
       </c>
-      <c r="E99" s="11">
+      <c r="E99" s="16">
         <v>35.2102429682582</v>
       </c>
-      <c r="F99" s="16">
+      <c r="F99" s="15">
         <v>710.81628148622599</v>
       </c>
       <c r="H99" s="13">
@@ -4915,13 +4918,13 @@
       <c r="C100" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="D100" s="16">
+      <c r="D100" s="13">
         <v>32.104103490651902</v>
       </c>
-      <c r="E100" s="11">
+      <c r="E100" s="16">
         <v>35.210095907450402</v>
       </c>
-      <c r="F100" s="16">
+      <c r="F100" s="15">
         <v>698.20619894878303</v>
       </c>
       <c r="H100" s="13">
@@ -4953,13 +4956,13 @@
       <c r="C101" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="D101" s="16">
+      <c r="D101" s="13">
         <v>32.104014359999901</v>
       </c>
-      <c r="E101" s="11">
+      <c r="E101" s="16">
         <v>35.210791514999997</v>
       </c>
-      <c r="F101" s="16">
+      <c r="F101" s="15">
         <v>697</v>
       </c>
       <c r="H101" s="13">
@@ -4991,13 +4994,13 @@
       <c r="C102" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="D102" s="16">
+      <c r="D102" s="13">
         <v>32.103724904733497</v>
       </c>
-      <c r="E102" s="11">
+      <c r="E102" s="16">
         <v>35.210207423797598</v>
       </c>
-      <c r="F102" s="16">
+      <c r="F102" s="15">
         <v>710.78306081931601</v>
       </c>
       <c r="H102" s="13">
@@ -5029,13 +5032,13 @@
       <c r="C103" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D103" s="16">
+      <c r="D103" s="13">
         <v>32.103724904733497</v>
       </c>
-      <c r="E103" s="11">
+      <c r="E103" s="16">
         <v>35.210207423797598</v>
       </c>
-      <c r="F103" s="16">
+      <c r="F103" s="15">
         <v>710.78306081931601</v>
       </c>
       <c r="H103" s="13">
@@ -5067,13 +5070,13 @@
       <c r="C104" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="D104" s="16">
+      <c r="D104" s="13">
         <v>32.103724904733497</v>
       </c>
-      <c r="E104" s="11">
+      <c r="E104" s="16">
         <v>35.210207423797598</v>
       </c>
-      <c r="F104" s="16">
+      <c r="F104" s="15">
         <v>710.78306081931601</v>
       </c>
       <c r="H104" s="13">
@@ -5105,13 +5108,13 @@
       <c r="C105" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="D105" s="16">
+      <c r="D105" s="13">
         <v>32.103804451692298</v>
       </c>
-      <c r="E105" s="11">
+      <c r="E105" s="16">
         <v>35.2102548886999</v>
       </c>
-      <c r="F105" s="16">
+      <c r="F105" s="15">
         <v>710.93479887847798</v>
       </c>
       <c r="H105" s="13">
@@ -5143,13 +5146,13 @@
       <c r="C106" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="D106" s="16">
+      <c r="D106" s="13">
         <v>32.102738363863097</v>
       </c>
-      <c r="E106" s="11">
+      <c r="E106" s="16">
         <v>35.209856687440301</v>
       </c>
-      <c r="F106" s="16">
+      <c r="F106" s="15">
         <v>711.90718361947904</v>
       </c>
       <c r="H106" s="13">
@@ -5181,13 +5184,13 @@
       <c r="C107" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="D107" s="16">
+      <c r="D107" s="13">
         <v>32.102689713395698</v>
       </c>
-      <c r="E107" s="11">
+      <c r="E107" s="16">
         <v>35.209867804165</v>
       </c>
-      <c r="F107" s="16">
+      <c r="F107" s="15">
         <v>711.897740273458</v>
       </c>
       <c r="H107" s="13">
@@ -5219,13 +5222,13 @@
       <c r="C108" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="D108" s="16">
+      <c r="D108" s="13">
         <v>32.102796625000003</v>
       </c>
-      <c r="E108" s="11">
+      <c r="E108" s="16">
         <v>35.208847085000002</v>
       </c>
-      <c r="F108" s="16">
+      <c r="F108" s="15">
         <v>687.5</v>
       </c>
       <c r="H108" s="13">
@@ -5257,13 +5260,13 @@
       <c r="C109" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="D109" s="16">
+      <c r="D109" s="13">
         <v>32.103630475334903</v>
       </c>
-      <c r="E109" s="11">
+      <c r="E109" s="16">
         <v>35.210050581227797</v>
       </c>
-      <c r="F109" s="16">
+      <c r="F109" s="15">
         <v>710.62788052011797</v>
       </c>
       <c r="H109" s="13">
@@ -5295,13 +5298,13 @@
       <c r="C110" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D110" s="16">
+      <c r="D110" s="13">
         <v>32.102930211930001</v>
       </c>
-      <c r="E110" s="11">
+      <c r="E110" s="16">
         <v>35.2096947789978</v>
       </c>
-      <c r="F110" s="16">
+      <c r="F110" s="15">
         <v>707.55191273982098</v>
       </c>
       <c r="H110" s="13">
@@ -5333,13 +5336,13 @@
       <c r="C111" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="D111" s="16">
+      <c r="D111" s="13">
         <v>32.102823390399799</v>
       </c>
-      <c r="E111" s="11">
+      <c r="E111" s="16">
         <v>35.209910451654402</v>
       </c>
-      <c r="F111" s="16">
+      <c r="F111" s="15">
         <v>705.83369046836503</v>
       </c>
       <c r="H111" s="13">
@@ -5371,13 +5374,13 @@
       <c r="C112" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="D112" s="16">
+      <c r="D112" s="13">
         <v>32.103724904733497</v>
       </c>
-      <c r="E112" s="11">
+      <c r="E112" s="16">
         <v>35.210207423797598</v>
       </c>
-      <c r="F112" s="16">
+      <c r="F112" s="15">
         <v>710.78306081931601</v>
       </c>
       <c r="H112" s="13">
@@ -5409,13 +5412,13 @@
       <c r="C113" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="D113" s="16">
+      <c r="D113" s="13">
         <v>32.102334680898601</v>
       </c>
-      <c r="E113" s="11">
+      <c r="E113" s="16">
         <v>35.209208439097999</v>
       </c>
-      <c r="F113" s="16">
+      <c r="F113" s="15">
         <v>688.910981725689</v>
       </c>
       <c r="H113" s="13">
@@ -5447,13 +5450,13 @@
       <c r="C114" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="D114" s="16">
+      <c r="D114" s="13">
         <v>32.104666270000003</v>
       </c>
-      <c r="E114" s="11">
+      <c r="E114" s="16">
         <v>35.209909359999997</v>
       </c>
-      <c r="F114" s="16">
+      <c r="F114" s="15">
         <v>687</v>
       </c>
       <c r="H114" s="13">
@@ -5485,13 +5488,13 @@
       <c r="C115" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="D115" s="16">
+      <c r="D115" s="13">
         <v>32.104642827968803</v>
       </c>
-      <c r="E115" s="11">
+      <c r="E115" s="16">
         <v>35.209878616465403</v>
       </c>
-      <c r="F115" s="16">
+      <c r="F115" s="15">
         <v>687.76145541783205</v>
       </c>
       <c r="H115" s="13">
@@ -5523,13 +5526,13 @@
       <c r="C116" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="D116" s="16">
+      <c r="D116" s="13">
         <v>32.102992868018397</v>
       </c>
-      <c r="E116" s="11">
+      <c r="E116" s="16">
         <v>35.208724744155099</v>
       </c>
-      <c r="F116" s="16">
+      <c r="F116" s="15">
         <v>686.14978935871397</v>
       </c>
       <c r="H116" s="13">
@@ -5561,13 +5564,13 @@
       <c r="C117" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="D117" s="16">
+      <c r="D117" s="13">
         <v>32.103515626049102</v>
       </c>
-      <c r="E117" s="11">
+      <c r="E117" s="16">
         <v>35.209225923213701</v>
       </c>
-      <c r="F117" s="16">
+      <c r="F117" s="15">
         <v>694.61525314947403</v>
       </c>
       <c r="H117" s="13">
@@ -5599,13 +5602,13 @@
       <c r="C118" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="D118" s="16">
+      <c r="D118" s="13">
         <v>32.1036628062297</v>
       </c>
-      <c r="E118" s="11">
+      <c r="E118" s="16">
         <v>35.209976951544803</v>
       </c>
-      <c r="F118" s="16">
+      <c r="F118" s="15">
         <v>711.15715212415603</v>
       </c>
       <c r="H118" s="13">
@@ -5637,13 +5640,13 @@
       <c r="C119" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="D119" s="16">
+      <c r="D119" s="13">
         <v>32.104123870000002</v>
       </c>
-      <c r="E119" s="11">
+      <c r="E119" s="16">
         <v>35.210913490000003</v>
       </c>
-      <c r="F119" s="16">
+      <c r="F119" s="15">
         <v>700</v>
       </c>
       <c r="H119" s="13">
@@ -5675,13 +5678,13 @@
       <c r="C120" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="D120" s="16">
+      <c r="D120" s="13">
         <v>32.102823620000002</v>
       </c>
-      <c r="E120" s="11">
+      <c r="E120" s="16">
         <v>35.208718990000001</v>
       </c>
-      <c r="F120" s="16">
+      <c r="F120" s="15">
         <v>688</v>
       </c>
       <c r="H120" s="13">
@@ -5713,13 +5716,13 @@
       <c r="C121" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="D121" s="16">
+      <c r="D121" s="13">
         <v>32.104004807260203</v>
       </c>
-      <c r="E121" s="11">
+      <c r="E121" s="16">
         <v>35.209208362652298</v>
       </c>
-      <c r="F121" s="16">
+      <c r="F121" s="15">
         <v>686.52955992443799</v>
       </c>
       <c r="H121" s="13">
@@ -5751,13 +5754,13 @@
       <c r="C122" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="D122" s="16">
+      <c r="D122" s="13">
         <v>32.104666270000003</v>
       </c>
-      <c r="E122" s="11">
+      <c r="E122" s="16">
         <v>35.209909359999997</v>
       </c>
-      <c r="F122" s="16">
+      <c r="F122" s="15">
         <v>687</v>
       </c>
       <c r="H122" s="13">
@@ -5789,13 +5792,13 @@
       <c r="C123" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D123" s="16">
+      <c r="D123" s="13">
         <v>32.104737513358799</v>
       </c>
-      <c r="E123" s="11">
+      <c r="E123" s="16">
         <v>35.210052631362998</v>
       </c>
-      <c r="F123" s="16">
+      <c r="F123" s="15">
         <v>687.408669527896</v>
       </c>
       <c r="H123" s="13">
@@ -5827,13 +5830,13 @@
       <c r="C124" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="D124" s="16">
+      <c r="D124" s="13">
         <v>32.102314229999998</v>
       </c>
-      <c r="E124" s="11">
+      <c r="E124" s="16">
         <v>35.209302194999999</v>
       </c>
-      <c r="F124" s="16">
+      <c r="F124" s="15">
         <v>690</v>
       </c>
       <c r="H124" s="13">
@@ -5865,13 +5868,13 @@
       <c r="C125" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="D125" s="16">
+      <c r="D125" s="13">
         <v>32.104402389999997</v>
       </c>
-      <c r="E125" s="11">
+      <c r="E125" s="16">
         <v>35.209460229999998</v>
       </c>
-      <c r="F125" s="16">
+      <c r="F125" s="15">
         <v>687</v>
       </c>
       <c r="H125" s="13">
@@ -5903,13 +5906,13 @@
       <c r="C126" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="D126" s="16">
+      <c r="D126" s="13">
         <v>32.104666270000003</v>
       </c>
-      <c r="E126" s="11">
+      <c r="E126" s="16">
         <v>35.209909359999997</v>
       </c>
-      <c r="F126" s="16">
+      <c r="F126" s="15">
         <v>687</v>
       </c>
       <c r="H126" s="13">
@@ -5941,13 +5944,13 @@
       <c r="C127" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="D127" s="16">
+      <c r="D127" s="13">
         <v>32.104790780103698</v>
       </c>
-      <c r="E127" s="11">
+      <c r="E127" s="16">
         <v>35.210154093438099</v>
       </c>
-      <c r="F127" s="16">
+      <c r="F127" s="15">
         <v>688.57152571185702</v>
       </c>
       <c r="H127" s="13">
@@ -5979,13 +5982,13 @@
       <c r="C128" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="D128" s="16">
+      <c r="D128" s="13">
         <v>32.104120940418703</v>
       </c>
-      <c r="E128" s="11">
+      <c r="E128" s="16">
         <v>35.209092718506703</v>
       </c>
-      <c r="F128" s="16">
+      <c r="F128" s="15">
         <v>685</v>
       </c>
       <c r="H128" s="13">
@@ -6017,13 +6020,13 @@
       <c r="C129" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="D129" s="16">
+      <c r="D129" s="13">
         <v>32.10406321</v>
       </c>
-      <c r="E129" s="11">
+      <c r="E129" s="16">
         <v>35.209027089999999</v>
       </c>
-      <c r="F129" s="16">
+      <c r="F129" s="15">
         <v>685</v>
       </c>
       <c r="H129" s="13">
@@ -6055,13 +6058,13 @@
       <c r="C130" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="D130" s="16">
+      <c r="D130" s="13">
         <v>32.10406321</v>
       </c>
-      <c r="E130" s="11">
+      <c r="E130" s="16">
         <v>35.209027089999999</v>
       </c>
-      <c r="F130" s="16">
+      <c r="F130" s="15">
         <v>685</v>
       </c>
       <c r="H130" s="13">
@@ -6093,13 +6096,13 @@
       <c r="C131" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="D131" s="16">
+      <c r="D131" s="13">
         <v>32.104521026007497</v>
       </c>
-      <c r="E131" s="11">
+      <c r="E131" s="16">
         <v>35.209724208152501</v>
       </c>
-      <c r="F131" s="16">
+      <c r="F131" s="15">
         <v>686.51818115037099</v>
       </c>
       <c r="H131" s="13">
@@ -6131,13 +6134,13 @@
       <c r="C132" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="D132" s="16">
+      <c r="D132" s="13">
         <v>32.104743295612501</v>
       </c>
-      <c r="E132" s="11">
+      <c r="E132" s="16">
         <v>35.210060920418599</v>
       </c>
-      <c r="F132" s="16">
+      <c r="F132" s="15">
         <v>687.94778005107696</v>
       </c>
       <c r="H132" s="13">
@@ -6169,13 +6172,13 @@
       <c r="C133" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="D133" s="16">
+      <c r="D133" s="13">
         <v>32.102600822128402</v>
       </c>
-      <c r="E133" s="11">
+      <c r="E133" s="16">
         <v>35.209431102770601</v>
       </c>
-      <c r="F133" s="16">
+      <c r="F133" s="15">
         <v>690.34862385321105</v>
       </c>
       <c r="H133" s="13">
@@ -6207,13 +6210,13 @@
       <c r="C134" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="D134" s="16">
+      <c r="D134" s="13">
         <v>32.103667998430502</v>
       </c>
-      <c r="E134" s="11">
+      <c r="E134" s="16">
         <v>35.2101723465546</v>
       </c>
-      <c r="F134" s="16">
+      <c r="F134" s="15">
         <v>699.87752574278295</v>
       </c>
       <c r="H134" s="13">
@@ -6245,13 +6248,13 @@
       <c r="C135" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="D135" s="16">
+      <c r="D135" s="13">
         <v>32.103763649999998</v>
       </c>
-      <c r="E135" s="11">
+      <c r="E135" s="16">
         <v>35.208836220000002</v>
       </c>
-      <c r="F135" s="16">
+      <c r="F135" s="15">
         <v>686</v>
       </c>
       <c r="H135" s="13">
@@ -6283,13 +6286,13 @@
       <c r="C136" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="D136" s="16">
+      <c r="D136" s="13">
         <v>32.102988115268303</v>
       </c>
-      <c r="E136" s="11">
+      <c r="E136" s="16">
         <v>35.209665175144998</v>
       </c>
-      <c r="F136" s="16">
+      <c r="F136" s="15">
         <v>702.04090298139101</v>
       </c>
       <c r="H136" s="13">
@@ -6321,13 +6324,13 @@
       <c r="C137" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="D137" s="16">
+      <c r="D137" s="13">
         <v>32.103295891783297</v>
       </c>
-      <c r="E137" s="11">
+      <c r="E137" s="16">
         <v>35.208819096421102</v>
       </c>
-      <c r="F137" s="16">
+      <c r="F137" s="15">
         <v>686</v>
       </c>
       <c r="H137" s="13">
@@ -6359,13 +6362,13 @@
       <c r="C138" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="D138" s="16">
+      <c r="D138" s="13">
         <v>32.102823620000002</v>
       </c>
-      <c r="E138" s="11">
+      <c r="E138" s="16">
         <v>35.208718990000001</v>
       </c>
-      <c r="F138" s="16">
+      <c r="F138" s="15">
         <v>688</v>
       </c>
       <c r="H138" s="13">
@@ -6397,13 +6400,13 @@
       <c r="C139" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="D139" s="16">
+      <c r="D139" s="13">
         <v>32.103073794228301</v>
       </c>
-      <c r="E139" s="11">
+      <c r="E139" s="16">
         <v>35.208807000377199</v>
       </c>
-      <c r="F139" s="16">
+      <c r="F139" s="15">
         <v>686.96640728432305</v>
       </c>
       <c r="H139" s="13">
@@ -6435,13 +6438,13 @@
       <c r="C140" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="D140" s="16">
+      <c r="D140" s="13">
         <v>32.102032199999996</v>
       </c>
-      <c r="E140" s="11">
+      <c r="E140" s="16">
         <v>35.209357019999999</v>
       </c>
-      <c r="F140" s="16">
+      <c r="F140" s="15">
         <v>688.99999999999898</v>
       </c>
       <c r="H140" s="13">
@@ -6473,13 +6476,13 @@
       <c r="C141" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="D141" s="16">
+      <c r="D141" s="13">
         <v>32.1036797538112</v>
       </c>
-      <c r="E141" s="11">
+      <c r="E141" s="16">
         <v>35.208948158369701</v>
       </c>
-      <c r="F141" s="16">
+      <c r="F141" s="15">
         <v>684.48823692222504</v>
       </c>
       <c r="H141" s="13">
@@ -6511,13 +6514,13 @@
       <c r="C142" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="D142" s="16">
+      <c r="D142" s="13">
         <v>32.102379398750202</v>
       </c>
-      <c r="E142" s="11">
+      <c r="E142" s="16">
         <v>35.209192027310998</v>
       </c>
-      <c r="F142" s="16">
+      <c r="F142" s="15">
         <v>689.38328049390896</v>
       </c>
       <c r="H142" s="13">
@@ -6549,13 +6552,13 @@
       <c r="C143" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="D143" s="16">
+      <c r="D143" s="13">
         <v>32.103841037977702</v>
       </c>
-      <c r="E143" s="11">
+      <c r="E143" s="16">
         <v>35.209019460784397</v>
       </c>
-      <c r="F143" s="16">
+      <c r="F143" s="15">
         <v>684.64886412344595</v>
       </c>
       <c r="H143" s="13">
@@ -6587,13 +6590,13 @@
       <c r="C144" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="D144" s="19">
+      <c r="D144" s="18">
         <v>32.1025033605884</v>
       </c>
-      <c r="E144" s="11">
+      <c r="E144" s="19">
         <v>35.209152684954098</v>
       </c>
-      <c r="F144" s="19">
+      <c r="F144" s="17">
         <v>689.93767795001497</v>
       </c>
       <c r="H144" s="18">
@@ -6619,25 +6622,25 @@
       </c>
     </row>
     <row r="145" spans="3:17" ht="31" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C145" s="34"/>
-      <c r="E145" s="34"/>
-      <c r="L145" s="20">
+      <c r="C145" s="20"/>
+      <c r="E145" s="37"/>
+      <c r="L145" s="23">
         <f>AVERAGE(L4:L144)</f>
-        <v>1.9055581291176239E-6</v>
+        <v>1.8939861878936155E-6</v>
       </c>
       <c r="M145" s="3">
         <f>AVERAGE(M4:M144)</f>
-        <v>1.9931161518064311E-6</v>
-      </c>
-      <c r="N145" s="21">
+        <v>1.9480875084991083E-6</v>
+      </c>
+      <c r="N145" s="24">
         <f>AVERAGE(N4:N144)</f>
-        <v>1.6364500000064407E-2</v>
-      </c>
-      <c r="O145" s="28" t="s">
+        <v>4.1039050095632905E-2</v>
+      </c>
+      <c r="O145" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="P145" s="29"/>
-      <c r="Q145" s="30"/>
+      <c r="P145" s="32"/>
+      <c r="Q145" s="33"/>
     </row>
     <row r="146" spans="3:17" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>

</xml_diff>